<commit_message>
added Messages -when Reserved & In Use tool becomes Free, user who reserved tool receives notification
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D6AE5C-383D-4A4D-914C-515B5A557FEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737E0741-9795-4DDF-ABD0-CE704F5BDD89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>resource_lang</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Sisse logimine</t>
   </si>
   <si>
-    <t>Регистрация</t>
-  </si>
-  <si>
     <t>login.username</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>Kasutajanimi</t>
   </si>
   <si>
-    <t>Рег. Имя</t>
-  </si>
-  <si>
     <t>login.password</t>
   </si>
   <si>
@@ -190,10 +184,10 @@
     <t>Logi sisse</t>
   </si>
   <si>
-    <t>login.select.caption</t>
-  </si>
-  <si>
-    <t>Select Account</t>
+    <t>Авторизация</t>
+  </si>
+  <si>
+    <t>Имя пользователя</t>
   </si>
 </sst>
 </file>
@@ -201,7 +195,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -275,7 +269,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -566,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,216 +629,199 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>